<commit_message>
The duration of each step should be longer than the length of the RGB pulse sets
</commit_message>
<xml_diff>
--- a/ledProtocols/protocolRGBTemplate.xlsx
+++ b/ledProtocols/protocolRGBTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (HHMI)\Current Projects\flyBowlRGB\FlyBowl4\ledProtocols\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (HHMI)\Current Projects\Katie\FlyBowl4\https---github.com-liujinyang-FlyBowl4Rig.git\ledProtocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F532FA51-7B4A-4B82-AF72-0D378DC74B5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93503B9B-32D0-49AA-AD51-C8C1086CF7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1305" yWindow="1170" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1002,7 +1002,7 @@
   <dimension ref="A1:CF3343"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1297,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="20">
-        <v>30000</v>
+        <v>35000</v>
       </c>
       <c r="C6" s="20">
         <v>2</v>

</xml_diff>